<commit_message>
added new column for data scraping
</commit_message>
<xml_diff>
--- a/EP2019_pest county_hungary.xlsx
+++ b/EP2019_pest county_hungary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="387">
   <si>
     <t>Abony</t>
   </si>
@@ -611,6 +611,570 @@
   </si>
   <si>
     <t>town_name</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=knQTGqwO&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=001&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=knQTGqwO&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=002&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=RNGX3Uze&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=003&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=RNGX3Uze&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=004&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=RNGX3Uze&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=005&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=RNGX3Uze&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=007&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=FRNM7bTa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=006&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=FRNM7bTa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=008&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=FRNM7bTa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=010&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=FRNM7bTa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=009&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=FRNM7bTa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=011&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VwHG5S5g&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=012&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VwHG5S5g&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=013&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VwHG5S5g&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=014&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=KhFwDoci&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=015&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=KhFwDoci&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=016&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=rBEKWpmi&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=017&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=62QkbIfs&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=018&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=62QkbIfs&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=019&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=62QkbIfs&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=020&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=62QkbIfs&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=021&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=62QkbIfs&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=022&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=CnZIR7qB&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=023&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=CnZIR7qB&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=185&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=CnZIR7qB&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=024&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mmy9Kpra&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=025&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mmy9Kpra&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=026&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mmy9Kpra&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=027&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mmy9Kpra&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=028&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=iSX7QJSq&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=029&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=iSX7QJSq&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=030&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=iSX7QJSq&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=031&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=iSX7QJSq&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=032&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DC8vNl1z&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=033&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DC8vNl1z&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=034&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=Qix57pXg&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=035&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=Qix57pXg&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=036&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=pw4gZ2k9&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=038&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=ItTAYY0K&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=037&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DGJXZ1sw&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=039&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DGJXZ1sw&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=040&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=hAWo2vXy&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=041&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=hAWo2vXy&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=042&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=hAWo2vXy&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=043&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=hAWo2vXy&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=044&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=hAWo2vXy&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=045&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=Rum6Q5o5&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=046&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=Rum6Q5o5&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=047&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=7Q9gJXks&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=048&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=7Q9gJXks&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=049&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=E8JfDKFc&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=050&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=6&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=051&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=052&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=053&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=054&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=055&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=056&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=XnmkCTUl&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=057&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LfKfUbA4&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=058&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LfKfUbA4&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=059&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LfKfUbA4&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=060&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LfKfUbA4&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=061&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LfKfUbA4&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=062&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=fvTLAFdk&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=063&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=fvTLAFdk&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=064&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=fvTLAFdk&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=065&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=fvTLAFdk&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=066&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=fvTLAFdk&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=067&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=fvTLAFdk&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=068&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=UqM255DD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=069&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=UqM255DD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=070&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=UqM255DD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=072&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=UqM255DD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=071&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=UqM255DD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=073&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=UqM255DD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=074&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=075&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=076&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=077&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=078&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=079&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=080&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=081&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=082&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yBCnTreR&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=083&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=L16pT4VD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=084&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=L16pT4VD&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=085&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EDLJMsYz&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=187&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EDLJMsYz&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=086&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EDLJMsYz&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=087&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EDLJMsYz&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=088&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=cibKgaL4&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=089&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yWr8URcb&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=090&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yWr8URcb&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=091&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yWr8URcb&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=092&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yWr8URcb&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=093&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=kyHWuxJ6&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=094&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=kyHWuxJ6&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=096&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=kyHWuxJ6&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=095&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=kyHWuxJ6&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=097&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=dnFKoS9U&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=098&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=dnFKoS9U&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=102&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EbnREnGp&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=099&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EbnREnGp&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=100&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EbnREnGp&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=101&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EbnREnGp&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=103&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EbnREnGp&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=104&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=EbnREnGp&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=105&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=106&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=107&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=112&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=108&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=109&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=110&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=VxRviJMI&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=111&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=AfTYUkJ1&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=114&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=AfTYUkJ1&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=113&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=115&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=116&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=117&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=118&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=119&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=120&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=9SdGE8oa&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=186&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=J2Yju9Ij&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=121&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=J2Yju9Ij&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=122&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=J2Yju9Ij&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=123&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=J2Yju9Ij&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=124&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=kKTn024o&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=125&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=kKTn024o&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=126&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=0ebHVcEM&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=127&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=0ebHVcEM&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=128&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=0ebHVcEM&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=129&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=0ebHVcEM&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=130&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=wYnjonAx&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=131&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=16&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=wYnjonAx&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=132&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=wYnjonAx&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=133&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=b3d92xW6&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=134&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=11&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DCf529bY&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=135&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DCf529bY&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=136&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DCf529bY&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=137&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=DCf529bY&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=138&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mvki41ic&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=139&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mvki41ic&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=143&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mvki41ic&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=140&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mvki41ic&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=141&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=mvki41ic&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=144&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TYGa4gW2&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=145&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TYGa4gW2&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=146&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TYGa4gW2&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=147&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TYGa4gW2&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=148&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=8Afp94rt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=149&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=8Afp94rt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=150&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=8Afp94rt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=151&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=8Afp94rt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=142&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=8Afp94rt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=152&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=NgRIjN3H&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=153&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=NgRIjN3H&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=154&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=NgRIjN3H&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=155&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=NgRIjN3H&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=156&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=NgRIjN3H&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=157&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yIeivMrB&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=158&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yIeivMrB&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=159&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=yIeivMrB&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=160&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=jWi4N1tn&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=161&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=jWi4N1tn&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=162&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=jWi4N1tn&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=163&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=jWi4N1tn&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=164&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=jWi4N1tn&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=165&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LNTeGmNt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=166&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=LNTeGmNt&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=169&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=lIkaxFSU&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=170&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=lIkaxFSU&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=171&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=lIkaxFSU&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=172&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TPRfdgrd&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=173&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TPRfdgrd&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=174&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TPRfdgrd&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=175&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TPRfdgrd&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=167&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TPRfdgrd&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=176&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TPRfdgrd&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=168&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=drNo20Ig&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=177&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=drNo20Ig&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=178&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=YRhfBLz0&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=179&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=YRhfBLz0&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=180&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=YRhfBLz0&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=181&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=YRhfBLz0&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=182&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=YRhfBLz0&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=183&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>http://www.valasztas.hu/szavazokorok_ep2019?p_p_auth=TZ5f4ux0&amp;p_p_id=epszavazokorieredmenyek_WAR_nvinvrportlet&amp;p_p_lifecycle=1&amp;p_p_state=maximized&amp;p_p_mode=view&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_valaltipKod=E&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_telepulesKod=184&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod2=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vlId=291&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_searchText=Somogy+megye&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_szavkorSorszam=1&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_megyeKod=14&amp;_epszavazokorieredmenyek_WAR_nvinvrportlet_vltId=684</t>
+  </si>
+  <si>
+    <t>one_voting_district_from_town</t>
   </si>
 </sst>
 </file>
@@ -663,12 +1227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -973,7 +1538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L189"/>
+  <dimension ref="A1:M189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -996,7 +1561,7 @@
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>198</v>
       </c>
@@ -1033,8 +1598,11 @@
       <c r="L1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1071,8 +1639,11 @@
       <c r="L2" s="1">
         <v>1.8549399777967548</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1109,8 +1680,11 @@
       <c r="L3" s="1">
         <v>1.1494252873563218</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1147,8 +1721,11 @@
       <c r="L4" s="1">
         <v>3.0893826147026431</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1185,8 +1762,11 @@
       <c r="L5" s="1">
         <v>2.0511044237965939</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1223,8 +1803,11 @@
       <c r="L6" s="1">
         <v>1.107011070110701</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1261,8 +1844,11 @@
       <c r="L7" s="1">
         <v>1.8229166666666667</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1299,8 +1885,11 @@
       <c r="L8" s="1">
         <v>3.1558641637711489</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1337,8 +1926,11 @@
       <c r="L9" s="1">
         <v>1.359492068652949</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1375,8 +1967,11 @@
       <c r="L10" s="1">
         <v>2.4038461538461542</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1413,8 +2008,11 @@
       <c r="L11" s="1">
         <v>1.9169329073482428</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1451,8 +2049,11 @@
       <c r="L12" s="1">
         <v>3.5727078857289651</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1489,8 +2090,11 @@
       <c r="L13" s="1">
         <v>3.6121601651380448</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1527,8 +2131,11 @@
       <c r="L14" s="1">
         <v>4.1280754592473361</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1565,8 +2172,11 @@
       <c r="L15" s="1">
         <v>3.8045053966930134</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1603,8 +2213,11 @@
       <c r="L16" s="1">
         <v>3.7917718092711694</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1641,8 +2254,11 @@
       <c r="L17" s="1">
         <v>1.7775499907515635</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1679,8 +2295,11 @@
       <c r="L18" s="1">
         <v>2.596466608273635</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1717,8 +2336,11 @@
       <c r="L19" s="1">
         <v>2.9249143777018589</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1755,8 +2377,11 @@
       <c r="L20" s="1">
         <v>1.6684002496359476</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1793,8 +2418,11 @@
       <c r="L21" s="1">
         <v>2.3483395053465994</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1831,8 +2459,11 @@
       <c r="L22" s="1">
         <v>6.1164537425058905</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1869,8 +2500,11 @@
       <c r="L23" s="1">
         <v>2.6548672566371683</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1907,8 +2541,11 @@
       <c r="L24" s="1">
         <v>3.3180603758132219</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>184</v>
       </c>
@@ -1945,8 +2582,11 @@
       <c r="L25" s="1">
         <v>3.106423777564717</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1983,8 +2623,11 @@
       <c r="L26" s="1">
         <v>1.7021276595744681</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2021,8 +2664,11 @@
       <c r="L27" s="1">
         <v>2.355978292976074</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -2059,8 +2705,11 @@
       <c r="L28" s="1">
         <v>1.8924449388889526</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2097,8 +2746,11 @@
       <c r="L29" s="1">
         <v>0.83288127706800263</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -2135,8 +2787,11 @@
       <c r="L30" s="1">
         <v>3.3723761771033995</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -2173,8 +2828,11 @@
       <c r="L31" s="1">
         <v>3.2326771752715469</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2211,8 +2869,11 @@
       <c r="L32" s="1">
         <v>1.7052455175615098</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2249,8 +2910,11 @@
       <c r="L33" s="1">
         <v>1.313498719010376</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -2287,8 +2951,11 @@
       <c r="L34" s="1">
         <v>1.4463830929179011</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -2325,8 +2992,11 @@
       <c r="L35" s="1">
         <v>3.6278423905320647</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2363,8 +3033,11 @@
       <c r="L36" s="1">
         <v>3.6475791094526357</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2401,8 +3074,11 @@
       <c r="L37" s="1">
         <v>3.5653677118248104</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2439,8 +3115,11 @@
       <c r="L38" s="1">
         <v>2.9029524792958608</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2477,8 +3156,11 @@
       <c r="L39" s="1">
         <v>3.3050286416189043</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2515,8 +3197,11 @@
       <c r="L40" s="1">
         <v>3.8574385855585334</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -2553,8 +3238,11 @@
       <c r="L41" s="1">
         <v>1.455437294997699</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2591,8 +3279,11 @@
       <c r="L42" s="1">
         <v>2.9511338335964736</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2629,8 +3320,11 @@
       <c r="L43" s="1">
         <v>3.1885834391576533</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2667,8 +3361,11 @@
       <c r="L44" s="1">
         <v>1.9886363636363635</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2705,8 +3402,11 @@
       <c r="L45" s="1">
         <v>1.0383264620552757</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2743,8 +3443,11 @@
       <c r="L46" s="1">
         <v>2.5549584758182706</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2781,8 +3484,11 @@
       <c r="L47" s="1">
         <v>4.7838789870404277</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -2819,8 +3525,11 @@
       <c r="L48" s="1">
         <v>4.0450184403523579</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2857,8 +3566,11 @@
       <c r="L49" s="1">
         <v>4.0763916454669067</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2895,8 +3607,11 @@
       <c r="L50" s="1">
         <v>3.0613385086539697</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2933,8 +3648,11 @@
       <c r="L51" s="1">
         <v>3.9015812841661104</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2971,8 +3689,11 @@
       <c r="L52" s="1">
         <v>3.0000588981752623</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -3009,8 +3730,11 @@
       <c r="L53" s="1">
         <v>4.2580984006505824</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -3047,8 +3771,11 @@
       <c r="L54" s="1">
         <v>2.2296367138565985</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -3085,8 +3812,11 @@
       <c r="L55" s="1">
         <v>2.4058509064216236</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -3123,8 +3853,11 @@
       <c r="L56" s="1">
         <v>2.4189774189774189</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -3161,8 +3894,11 @@
       <c r="L57" s="1">
         <v>2.2479511137045964</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -3199,8 +3935,11 @@
       <c r="L58" s="1">
         <v>2.7777777777777777</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -3237,8 +3976,11 @@
       <c r="L59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -3275,8 +4017,11 @@
       <c r="L60" s="1">
         <v>3.5556778590781373</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -3313,8 +4058,11 @@
       <c r="L61" s="1">
         <v>1.6926044080496216</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -3351,8 +4099,11 @@
       <c r="L62" s="1">
         <v>2.6665641688703299</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -3389,8 +4140,11 @@
       <c r="L63" s="1">
         <v>1.7851196169763917</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -3427,8 +4181,11 @@
       <c r="L64" s="1">
         <v>2.7649769585253456</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -3465,8 +4222,11 @@
       <c r="L65" s="1">
         <v>2.8708133971291865</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -3503,8 +4263,11 @@
       <c r="L66" s="1">
         <v>3.1991076517500505</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -3541,8 +4304,11 @@
       <c r="L67" s="1">
         <v>1.818399256648634</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -3579,8 +4345,11 @@
       <c r="L68" s="1">
         <v>3.4969545442455514</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -3617,8 +4386,11 @@
       <c r="L69" s="1">
         <v>0.82304526748971196</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M69" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -3655,8 +4427,11 @@
       <c r="L70" s="1">
         <v>2.9661016949152543</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -3693,8 +4468,11 @@
       <c r="L71" s="1">
         <v>3.4336196667958485</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -3731,8 +4509,11 @@
       <c r="L72" s="1">
         <v>1.5536263338759271</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -3769,8 +4550,11 @@
       <c r="L73" s="1">
         <v>2.5005336277728882</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -3807,8 +4591,11 @@
       <c r="L74" s="1">
         <v>4.5031761487457684</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -3845,8 +4632,11 @@
       <c r="L75" s="1">
         <v>3.1141868512110724</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -3883,8 +4673,11 @@
       <c r="L76" s="1">
         <v>0.74074074074074081</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M76" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -3921,8 +4714,11 @@
       <c r="L77" s="1">
         <v>5.2632200307608983</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M77" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -3959,8 +4755,11 @@
       <c r="L78" s="1">
         <v>1.1494252873563218</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M78" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -3997,8 +4796,11 @@
       <c r="L79" s="1">
         <v>0.86206896551724133</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M79" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -4035,8 +4837,11 @@
       <c r="L80" s="1">
         <v>3.046307785425117</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M80" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -4073,8 +4878,11 @@
       <c r="L81" s="1">
         <v>1.800327332242226</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -4111,8 +4919,11 @@
       <c r="L82" s="1">
         <v>1.0899182561307901</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M82" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -4149,8 +4960,11 @@
       <c r="L83" s="1">
         <v>1.1152416356877324</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M83" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -4187,8 +5001,11 @@
       <c r="L84" s="1">
         <v>3.2951599405370695</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M84" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -4225,8 +5042,11 @@
       <c r="L85" s="1">
         <v>2.1390374331550799</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M85" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -4263,8 +5083,11 @@
       <c r="L86" s="1">
         <v>2.2362784929423043</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M86" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -4301,8 +5124,11 @@
       <c r="L87" s="1">
         <v>3.1630685134421257</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M87" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>186</v>
       </c>
@@ -4339,8 +5165,11 @@
       <c r="L88" s="1">
         <v>3.9275427230586599</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -4377,8 +5206,11 @@
       <c r="L89" s="1">
         <v>1.6129032258064515</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -4415,8 +5247,11 @@
       <c r="L90" s="1">
         <v>2.1471434788890096</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M90" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -4453,8 +5288,11 @@
       <c r="L91" s="1">
         <v>5.077927081100241</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M91" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -4491,8 +5329,11 @@
       <c r="L92" s="1">
         <v>1.8865876554618812</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M92" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -4529,8 +5370,11 @@
       <c r="L93" s="1">
         <v>3.8541790774464819</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M93" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -4567,8 +5411,11 @@
       <c r="L94" s="1">
         <v>4.1861282774685673</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M94" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -4605,8 +5452,11 @@
       <c r="L95" s="1">
         <v>1.6659707836178426</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M95" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>92</v>
       </c>
@@ -4643,8 +5493,11 @@
       <c r="L96" s="1">
         <v>2.3710515793682529</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M96" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -4681,8 +5534,11 @@
       <c r="L97" s="1">
         <v>2.8021304087638224</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M97" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -4719,8 +5575,11 @@
       <c r="L98" s="1">
         <v>3.7876378178503414</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M98" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>94</v>
       </c>
@@ -4757,8 +5616,11 @@
       <c r="L99" s="1">
         <v>1.9215301193652619</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M99" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>96</v>
       </c>
@@ -4795,8 +5657,11 @@
       <c r="L100" s="1">
         <v>2.4747474747474749</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M100" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -4833,8 +5698,11 @@
       <c r="L101" s="1">
         <v>3.9006525814072566</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M101" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -4871,8 +5739,11 @@
       <c r="L102" s="1">
         <v>3.2878944947912245</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M102" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>98</v>
       </c>
@@ -4909,8 +5780,11 @@
       <c r="L103" s="1">
         <v>2.1194605009633909</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M103" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>99</v>
       </c>
@@ -4947,8 +5821,11 @@
       <c r="L104" s="1">
         <v>3.0956771709063293</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M104" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>100</v>
       </c>
@@ -4985,8 +5862,11 @@
       <c r="L105" s="1">
         <v>2.4096385542168677</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M105" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -5023,8 +5903,11 @@
       <c r="L106" s="1">
         <v>3.5465768799102131</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M106" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -5061,8 +5944,11 @@
       <c r="L107" s="1">
         <v>3.0204130166861018</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M107" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>104</v>
       </c>
@@ -5099,8 +5985,11 @@
       <c r="L108" s="1">
         <v>6.4204426838100233</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M108" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>105</v>
       </c>
@@ -5137,8 +6026,11 @@
       <c r="L109" s="1">
         <v>4.3454250056728254</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M109" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>106</v>
       </c>
@@ -5175,8 +6067,11 @@
       <c r="L110" s="1">
         <v>5.6179775280898872</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M110" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -5213,8 +6108,11 @@
       <c r="L111" s="1">
         <v>2.7356418032006733</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M111" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -5251,8 +6149,11 @@
       <c r="L112" s="1">
         <v>3.0749095073518884</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M112" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>108</v>
       </c>
@@ -5289,8 +6190,11 @@
       <c r="L113" s="1">
         <v>3.88007492413238</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M113" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>109</v>
       </c>
@@ -5327,8 +6231,11 @@
       <c r="L114" s="1">
         <v>3.8098642606839328</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M114" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>110</v>
       </c>
@@ -5365,8 +6272,11 @@
       <c r="L115" s="1">
         <v>5.6511056511056514</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M115" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -5403,8 +6313,11 @@
       <c r="L116" s="1">
         <v>3.4304740957966766</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M116" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>112</v>
       </c>
@@ -5441,8 +6354,11 @@
       <c r="L117" s="1">
         <v>4.5551863456909301</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M117" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -5479,8 +6395,11 @@
       <c r="L118" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M118" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -5517,8 +6436,11 @@
       <c r="L119" s="1">
         <v>3.9893617021276597</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M119" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -5555,8 +6477,11 @@
       <c r="L120" s="1">
         <v>1.1342155009451798</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M120" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -5593,8 +6518,11 @@
       <c r="L121" s="1">
         <v>2.1428571428571428</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M121" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -5631,8 +6559,11 @@
       <c r="L122" s="1">
         <v>2.1439486535651255</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M122" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -5669,8 +6600,11 @@
       <c r="L123" s="1">
         <v>2.5751072961373391</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M123" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>185</v>
       </c>
@@ -5707,8 +6641,11 @@
       <c r="L124" s="1">
         <v>5.040322580645161</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M124" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>120</v>
       </c>
@@ -5745,8 +6682,11 @@
       <c r="L125" s="1">
         <v>3.6982647978973886</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M125" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>121</v>
       </c>
@@ -5783,8 +6723,11 @@
       <c r="L126" s="1">
         <v>3.8245608196754106</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M126" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>122</v>
       </c>
@@ -5821,8 +6764,11 @@
       <c r="L127" s="1">
         <v>2.7917811733291757</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M127" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>123</v>
       </c>
@@ -5859,8 +6805,11 @@
       <c r="L128" s="1">
         <v>2.7130691370058742</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M128" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -5897,8 +6846,11 @@
       <c r="L129" s="1">
         <v>3.2192634866414425</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M129" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>125</v>
       </c>
@@ -5935,8 +6887,11 @@
       <c r="L130" s="1">
         <v>4.8532940044360782</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M130" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>126</v>
       </c>
@@ -5973,8 +6928,11 @@
       <c r="L131" s="1">
         <v>1.1041857501294357</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M131" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>127</v>
       </c>
@@ -6011,8 +6969,11 @@
       <c r="L132" s="1">
         <v>2.2785027297475837</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M132" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>128</v>
       </c>
@@ -6049,8 +7010,11 @@
       <c r="L133" s="1">
         <v>2.4096385542168677</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M133" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>129</v>
       </c>
@@ -6087,8 +7051,11 @@
       <c r="L134" s="1">
         <v>1.8498343842505474</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M134" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>130</v>
       </c>
@@ -6125,8 +7092,11 @@
       <c r="L135" s="1">
         <v>3.1255436511190369</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M135" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>131</v>
       </c>
@@ -6163,8 +7133,11 @@
       <c r="L136" s="1">
         <v>5.223046139359699</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M136" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>132</v>
       </c>
@@ -6201,8 +7174,11 @@
       <c r="L137" s="1">
         <v>2.4724524675381403</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M137" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>133</v>
       </c>
@@ -6239,8 +7215,11 @@
       <c r="L138" s="1">
         <v>3.2594629799693013</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M138" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>134</v>
       </c>
@@ -6277,8 +7256,11 @@
       <c r="L139" s="1">
         <v>2.9002849002849005</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M139" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>135</v>
       </c>
@@ -6315,8 +7297,11 @@
       <c r="L140" s="1">
         <v>1.5472981243152393</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M140" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>136</v>
       </c>
@@ -6353,8 +7338,11 @@
       <c r="L141" s="1">
         <v>3.5328177711140487</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M141" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>137</v>
       </c>
@@ -6391,8 +7379,11 @@
       <c r="L142" s="1">
         <v>2.2855557259377717</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M142" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -6429,8 +7420,11 @@
       <c r="L143" s="1">
         <v>3.3411137323465936</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M143" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -6467,8 +7461,11 @@
       <c r="L144" s="1">
         <v>1.4878359945522301</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M144" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>139</v>
       </c>
@@ -6505,8 +7502,11 @@
       <c r="L145" s="1">
         <v>3.929066953867685</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M145" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>140</v>
       </c>
@@ -6543,8 +7543,11 @@
       <c r="L146" s="1">
         <v>3.402704761399383</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M146" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>143</v>
       </c>
@@ -6581,8 +7584,11 @@
       <c r="L147" s="1">
         <v>1.6677865785464772</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M147" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>144</v>
       </c>
@@ -6619,8 +7625,11 @@
       <c r="L148" s="1">
         <v>0.98548693456864789</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M148" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -6657,8 +7666,11 @@
       <c r="L149" s="1">
         <v>1.4505881478358542</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M149" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>146</v>
       </c>
@@ -6695,8 +7707,11 @@
       <c r="L150" s="1">
         <v>2.0351707073414285</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M150" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>147</v>
       </c>
@@ -6733,8 +7748,11 @@
       <c r="L151" s="1">
         <v>2.3900314055604857</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M151" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>148</v>
       </c>
@@ -6771,8 +7789,11 @@
       <c r="L152" s="1">
         <v>1.3233197684663363</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M152" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>149</v>
       </c>
@@ -6809,8 +7830,11 @@
       <c r="L153" s="1">
         <v>1.0953413330644348</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M153" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>150</v>
       </c>
@@ -6847,8 +7871,11 @@
       <c r="L154" s="1">
         <v>3.8343378890312585</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M154" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>141</v>
       </c>
@@ -6885,8 +7912,11 @@
       <c r="L155" s="1">
         <v>1.5485021241002839</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M155" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>151</v>
       </c>
@@ -6923,8 +7953,11 @@
       <c r="L156" s="1">
         <v>5.0256621501829928</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M156" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -6961,8 +7994,11 @@
       <c r="L157" s="1">
         <v>8.1632653061224492</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M157" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>153</v>
       </c>
@@ -6999,8 +8035,11 @@
       <c r="L158" s="1">
         <v>4.9916805324459235</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M158" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>154</v>
       </c>
@@ -7037,8 +8076,11 @@
       <c r="L159" s="1">
         <v>1.6729937589070716</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M159" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>155</v>
       </c>
@@ -7075,8 +8117,11 @@
       <c r="L160" s="1">
         <v>2.6465028355387523</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M160" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>156</v>
       </c>
@@ -7113,8 +8158,11 @@
       <c r="L161" s="1">
         <v>3.0415503784737612</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M161" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>157</v>
       </c>
@@ -7151,8 +8199,11 @@
       <c r="L162" s="1">
         <v>3.2929433046132366</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M162" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>158</v>
       </c>
@@ -7189,8 +8240,11 @@
       <c r="L163" s="1">
         <v>1.9046193913892229</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M163" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>159</v>
       </c>
@@ -7227,8 +8281,11 @@
       <c r="L164" s="1">
         <v>2.5269117734152235</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M164" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>160</v>
       </c>
@@ -7265,8 +8322,11 @@
       <c r="L165" s="1">
         <v>1.4984243076939514</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M165" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>161</v>
       </c>
@@ -7303,8 +8363,11 @@
       <c r="L166" s="1">
         <v>1.015784494348454</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M166" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>162</v>
       </c>
@@ -7341,8 +8404,11 @@
       <c r="L167" s="1">
         <v>0.63059063404367266</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M167" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>163</v>
       </c>
@@ -7379,8 +8445,11 @@
       <c r="L168" s="1">
         <v>2.5799696927951508</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M168" s="5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>164</v>
       </c>
@@ -7417,8 +8486,11 @@
       <c r="L169" s="1">
         <v>2.8345698969655659</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M169" s="5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>165</v>
       </c>
@@ -7455,8 +8527,11 @@
       <c r="L170" s="1">
         <v>3.91610282286686</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M170" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>168</v>
       </c>
@@ -7493,8 +8568,11 @@
       <c r="L171" s="1">
         <v>2.5754260781978009</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M171" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>169</v>
       </c>
@@ -7531,8 +8609,11 @@
       <c r="L172" s="1">
         <v>5.244122965641953</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M172" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>170</v>
       </c>
@@ -7569,8 +8650,11 @@
       <c r="L173" s="1">
         <v>2.3346303501945527</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M173" s="5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>171</v>
       </c>
@@ -7607,8 +8691,11 @@
       <c r="L174" s="1">
         <v>3.1708981708981705</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M174" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>172</v>
       </c>
@@ -7645,8 +8732,11 @@
       <c r="L175" s="1">
         <v>2.1739130434782608</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M175" s="5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>173</v>
       </c>
@@ -7683,8 +8773,11 @@
       <c r="L176" s="1">
         <v>4.0163338809553899</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M176" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>174</v>
       </c>
@@ -7721,8 +8814,11 @@
       <c r="L177" s="1">
         <v>2.5520077406869861</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M177" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>166</v>
       </c>
@@ -7759,8 +8855,11 @@
       <c r="L178" s="1">
         <v>2.0158179012345681</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M178" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>175</v>
       </c>
@@ -7797,8 +8896,11 @@
       <c r="L179" s="1">
         <v>1.9802231237322514</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M179" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>167</v>
       </c>
@@ -7835,8 +8937,11 @@
       <c r="L180" s="1">
         <v>2.7748818459827631</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M180" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>176</v>
       </c>
@@ -7873,8 +8978,11 @@
       <c r="L181" s="1">
         <v>2.9872640222674742</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M181" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>177</v>
       </c>
@@ -7911,8 +9019,11 @@
       <c r="L182" s="1">
         <v>3.8415012646812108</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M182" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>178</v>
       </c>
@@ -7949,8 +9060,11 @@
       <c r="L183" s="1">
         <v>5.2202282877919863</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M183" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>179</v>
       </c>
@@ -7987,8 +9101,11 @@
       <c r="L184" s="1">
         <v>0.52083333333333326</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M184" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>180</v>
       </c>
@@ -8025,8 +9142,11 @@
       <c r="L185" s="1">
         <v>2.0271089379831091</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M185" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>181</v>
       </c>
@@ -8063,8 +9183,11 @@
       <c r="L186" s="1">
         <v>3.0405405405405408</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M186" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>182</v>
       </c>
@@ -8101,8 +9224,11 @@
       <c r="L187" s="1">
         <v>2.4550688595040002</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M187" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -8139,8 +9265,11 @@
       <c r="L188" s="1">
         <v>3.0633773683775063</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M188" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>

</xml_diff>